<commit_message>
Update df for analysis with NiiStat
</commit_message>
<xml_diff>
--- a/RData/data_acc_cond.xlsx
+++ b/RData/data_acc_cond.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -375,15 +375,10 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>lesion_volume</t>
+          <t>WPM</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>WPM</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>FPM</t>
         </is>
@@ -402,12 +397,9 @@
         <v>823.4285714285714</v>
       </c>
       <c r="D2">
-        <v>80497</v>
+        <v>0.7552083333333334</v>
       </c>
       <c r="E2">
-        <v>0.7552083333333334</v>
-      </c>
-      <c r="F2">
         <v>0.6190476190476191</v>
       </c>
     </row>
@@ -424,12 +416,9 @@
         <v>185.2857142857143</v>
       </c>
       <c r="D3">
-        <v>23285</v>
+        <v>0.2670157068062827</v>
       </c>
       <c r="E3">
-        <v>0.2670157068062827</v>
-      </c>
-      <c r="F3">
         <v>0.2894736842105263</v>
       </c>
     </row>
@@ -446,12 +435,9 @@
         <v>280.8571428571428</v>
       </c>
       <c r="D4">
-        <v>10727</v>
+        <v>0.8</v>
       </c>
       <c r="E4">
-        <v>0.8</v>
-      </c>
-      <c r="F4">
         <v>0.7671957671957672</v>
       </c>
     </row>
@@ -468,12 +454,9 @@
         <v>334.4285714285714</v>
       </c>
       <c r="D5">
-        <v>90943</v>
+        <v>0.08376963350785341</v>
       </c>
       <c r="E5">
-        <v>0.08376963350785341</v>
-      </c>
-      <c r="F5">
         <v>0.3315508021390374</v>
       </c>
     </row>
@@ -490,12 +473,9 @@
         <v>509.2857142857143</v>
       </c>
       <c r="D6">
-        <v>37855</v>
+        <v>0.9166666666666666</v>
       </c>
       <c r="E6">
-        <v>0.9166666666666666</v>
-      </c>
-      <c r="F6">
         <v>0.8138297872340425</v>
       </c>
     </row>
@@ -512,12 +492,9 @@
         <v>516.8571428571429</v>
       </c>
       <c r="D7">
-        <v>84355</v>
+        <v>0.4157894736842105</v>
       </c>
       <c r="E7">
-        <v>0.4157894736842105</v>
-      </c>
-      <c r="F7">
         <v>0.4117647058823529</v>
       </c>
     </row>
@@ -534,12 +511,9 @@
         <v>337.2857142857143</v>
       </c>
       <c r="D8">
-        <v>32445</v>
+        <v>0.5789473684210527</v>
       </c>
       <c r="E8">
-        <v>0.5789473684210527</v>
-      </c>
-      <c r="F8">
         <v>0.5578947368421052</v>
       </c>
     </row>
@@ -556,12 +530,9 @@
         <v>469.2857142857143</v>
       </c>
       <c r="D9">
-        <v>426250</v>
+        <v>0.06914893617021277</v>
       </c>
       <c r="E9">
-        <v>0.06914893617021277</v>
-      </c>
-      <c r="F9">
         <v>0.1555555555555556</v>
       </c>
     </row>
@@ -578,12 +549,9 @@
         <v>31.28571428571428</v>
       </c>
       <c r="D10">
-        <v>93057</v>
+        <v>0.5585106382978723</v>
       </c>
       <c r="E10">
-        <v>0.5585106382978723</v>
-      </c>
-      <c r="F10">
         <v>0.5133689839572193</v>
       </c>
     </row>
@@ -600,12 +568,9 @@
         <v>331.1428571428572</v>
       </c>
       <c r="D11">
-        <v>38515</v>
+        <v>0.3842105263157894</v>
       </c>
       <c r="E11">
-        <v>0.3842105263157894</v>
-      </c>
-      <c r="F11">
         <v>0.3541666666666667</v>
       </c>
     </row>
@@ -622,12 +587,9 @@
         <v>1422.428571428571</v>
       </c>
       <c r="D12">
-        <v>159574</v>
+        <v>0.7553191489361702</v>
       </c>
       <c r="E12">
-        <v>0.7553191489361702</v>
-      </c>
-      <c r="F12">
         <v>0.6424581005586593</v>
       </c>
     </row>
@@ -644,12 +606,9 @@
         <v>239.7142857142857</v>
       </c>
       <c r="D13">
-        <v>161280</v>
+        <v>0.5276073619631901</v>
       </c>
       <c r="E13">
-        <v>0.5276073619631901</v>
-      </c>
-      <c r="F13">
         <v>0.4903225806451613</v>
       </c>
     </row>
@@ -666,12 +625,9 @@
         <v>450.8571428571428</v>
       </c>
       <c r="D14">
-        <v>53638</v>
+        <v>0.9895833333333334</v>
       </c>
       <c r="E14">
-        <v>0.9895833333333334</v>
-      </c>
-      <c r="F14">
         <v>0.8677248677248677</v>
       </c>
     </row>
@@ -688,12 +644,9 @@
         <v>443.1428571428572</v>
       </c>
       <c r="D15">
-        <v>113765</v>
+        <v>0.203125</v>
       </c>
       <c r="E15">
-        <v>0.203125</v>
-      </c>
-      <c r="F15">
         <v>0.25</v>
       </c>
     </row>
@@ -710,12 +663,9 @@
         <v>405.5714285714286</v>
       </c>
       <c r="D16">
-        <v>46460</v>
+        <v>0.7684210526315789</v>
       </c>
       <c r="E16">
-        <v>0.7684210526315789</v>
-      </c>
-      <c r="F16">
         <v>0.7315789473684211</v>
       </c>
     </row>
@@ -732,14 +682,11 @@
         <v>179.8571428571429</v>
       </c>
       <c r="D17">
-        <v>60757</v>
+        <v>0.5210526315789473</v>
       </c>
       <c r="E17">
         <v>0.5210526315789473</v>
       </c>
-      <c r="F17">
-        <v>0.5210526315789473</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -754,12 +701,9 @@
         <v>202.7142857142857</v>
       </c>
       <c r="D18">
-        <v>124042</v>
+        <v>0.8201058201058201</v>
       </c>
       <c r="E18">
-        <v>0.8201058201058201</v>
-      </c>
-      <c r="F18">
         <v>0.7819148936170213</v>
       </c>
     </row>
@@ -776,12 +720,9 @@
         <v>141.7142857142857</v>
       </c>
       <c r="D19">
-        <v>51685</v>
+        <v>0.02604166666666667</v>
       </c>
       <c r="E19">
-        <v>0.02604166666666667</v>
-      </c>
-      <c r="F19">
         <v>0.1368421052631579</v>
       </c>
     </row>
@@ -798,12 +739,9 @@
         <v>275</v>
       </c>
       <c r="D20">
-        <v>33649</v>
+        <v>0.7894736842105263</v>
       </c>
       <c r="E20">
-        <v>0.7894736842105263</v>
-      </c>
-      <c r="F20">
         <v>0.7604166666666666</v>
       </c>
     </row>
@@ -820,12 +758,9 @@
         <v>555.8571428571429</v>
       </c>
       <c r="D21">
-        <v>94032</v>
+        <v>0.1675392670157068</v>
       </c>
       <c r="E21">
-        <v>0.1675392670157068</v>
-      </c>
-      <c r="F21">
         <v>0.2052631578947368</v>
       </c>
     </row>
@@ -842,12 +777,9 @@
         <v>843.2857142857143</v>
       </c>
       <c r="D22">
-        <v>164920</v>
+        <v>0.7777777777777778</v>
       </c>
       <c r="E22">
-        <v>0.7777777777777778</v>
-      </c>
-      <c r="F22">
         <v>0.6770833333333334</v>
       </c>
     </row>
@@ -864,12 +796,9 @@
         <v>146.2857142857143</v>
       </c>
       <c r="D23">
-        <v>84257</v>
+        <v>0.8952879581151832</v>
       </c>
       <c r="E23">
-        <v>0.8952879581151832</v>
-      </c>
-      <c r="F23">
         <v>0.8663101604278075</v>
       </c>
     </row>
@@ -886,12 +815,9 @@
         <v>162.2857142857143</v>
       </c>
       <c r="D24">
-        <v>28230</v>
+        <v>0.734375</v>
       </c>
       <c r="E24">
-        <v>0.734375</v>
-      </c>
-      <c r="F24">
         <v>0.7120418848167539</v>
       </c>
     </row>
@@ -908,12 +834,9 @@
         <v>481.5714285714286</v>
       </c>
       <c r="D25">
-        <v>246035</v>
+        <v>0.531578947368421</v>
       </c>
       <c r="E25">
-        <v>0.531578947368421</v>
-      </c>
-      <c r="F25">
         <v>0.4764397905759162</v>
       </c>
     </row>
@@ -930,12 +853,9 @@
         <v>128.5714285714286</v>
       </c>
       <c r="D26">
-        <v>23763</v>
+        <v>0.774869109947644</v>
       </c>
       <c r="E26">
-        <v>0.774869109947644</v>
-      </c>
-      <c r="F26">
         <v>0.6613756613756614</v>
       </c>
     </row>
@@ -952,12 +872,9 @@
         <v>131.4285714285714</v>
       </c>
       <c r="D27">
-        <v>8264</v>
+        <v>0.6596858638743456</v>
       </c>
       <c r="E27">
-        <v>0.6596858638743456</v>
-      </c>
-      <c r="F27">
         <v>0.7225130890052356</v>
       </c>
     </row>
@@ -974,12 +891,9 @@
         <v>436.4285714285714</v>
       </c>
       <c r="D28">
-        <v>15893</v>
+        <v>0.680628272251309</v>
       </c>
       <c r="E28">
-        <v>0.680628272251309</v>
-      </c>
-      <c r="F28">
         <v>0.6210526315789474</v>
       </c>
     </row>
@@ -996,12 +910,9 @@
         <v>121.5714285714286</v>
       </c>
       <c r="D29">
-        <v>1130</v>
+        <v>0.5668449197860963</v>
       </c>
       <c r="E29">
-        <v>0.5668449197860963</v>
-      </c>
-      <c r="F29">
         <v>0.6243386243386243</v>
       </c>
     </row>
@@ -1018,12 +929,9 @@
         <v>308</v>
       </c>
       <c r="D30">
-        <v>79200</v>
+        <v>0.8105263157894737</v>
       </c>
       <c r="E30">
-        <v>0.8105263157894737</v>
-      </c>
-      <c r="F30">
         <v>0.6894736842105263</v>
       </c>
     </row>
@@ -1040,12 +948,9 @@
         <v>96.71428571428571</v>
       </c>
       <c r="D31">
-        <v>20761</v>
+        <v>0.6701570680628273</v>
       </c>
       <c r="E31">
-        <v>0.6701570680628273</v>
-      </c>
-      <c r="F31">
         <v>0.6117021276595744</v>
       </c>
     </row>
@@ -1062,12 +967,9 @@
         <v>107.5714285714286</v>
       </c>
       <c r="D32">
-        <v>82699</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E32">
-        <v>0.6666666666666666</v>
-      </c>
-      <c r="F32">
         <v>0.6031746031746031</v>
       </c>
     </row>
@@ -1084,12 +986,9 @@
         <v>331.5714285714286</v>
       </c>
       <c r="D33">
-        <v>112356</v>
+        <v>0.7513227513227513</v>
       </c>
       <c r="E33">
-        <v>0.7513227513227513</v>
-      </c>
-      <c r="F33">
         <v>0.601063829787234</v>
       </c>
     </row>
@@ -1106,12 +1005,9 @@
         <v>161.7142857142857</v>
       </c>
       <c r="D34">
-        <v>50491</v>
+        <v>0.7368421052631579</v>
       </c>
       <c r="E34">
-        <v>0.7368421052631579</v>
-      </c>
-      <c r="F34">
         <v>0.6648351648351648</v>
       </c>
     </row>
@@ -1128,12 +1024,9 @@
         <v>229.8571428571429</v>
       </c>
       <c r="D35">
-        <v>67501</v>
+        <v>0.6631578947368421</v>
       </c>
       <c r="E35">
-        <v>0.6631578947368421</v>
-      </c>
-      <c r="F35">
         <v>0.6210526315789474</v>
       </c>
     </row>
@@ -1150,12 +1043,9 @@
         <v>196.7142857142857</v>
       </c>
       <c r="D36">
-        <v>25964</v>
+        <v>0.8109756097560976</v>
       </c>
       <c r="E36">
-        <v>0.8109756097560976</v>
-      </c>
-      <c r="F36">
         <v>0.632</v>
       </c>
     </row>
@@ -1172,12 +1062,9 @@
         <v>390.1428571428572</v>
       </c>
       <c r="D37">
-        <v>42050</v>
+        <v>0.8697916666666666</v>
       </c>
       <c r="E37">
-        <v>0.8697916666666666</v>
-      </c>
-      <c r="F37">
         <v>0.8157894736842105</v>
       </c>
     </row>
@@ -1194,12 +1081,9 @@
         <v>137.2857142857143</v>
       </c>
       <c r="D38">
-        <v>46698</v>
+        <v>0.78125</v>
       </c>
       <c r="E38">
-        <v>0.78125</v>
-      </c>
-      <c r="F38">
         <v>0.7120418848167539</v>
       </c>
     </row>
@@ -1216,12 +1100,9 @@
         <v>1061</v>
       </c>
       <c r="D39">
-        <v>149943</v>
+        <v>0.6842105263157895</v>
       </c>
       <c r="E39">
-        <v>0.6842105263157895</v>
-      </c>
-      <c r="F39">
         <v>0.6421052631578947</v>
       </c>
     </row>
@@ -1238,12 +1119,9 @@
         <v>79.14285714285714</v>
       </c>
       <c r="D40">
-        <v>79825</v>
+        <v>0.746031746031746</v>
       </c>
       <c r="E40">
-        <v>0.746031746031746</v>
-      </c>
-      <c r="F40">
         <v>0.6455026455026455</v>
       </c>
     </row>
@@ -1260,12 +1138,9 @@
         <v>95.85714285714286</v>
       </c>
       <c r="D41">
-        <v>150679</v>
+        <v>0.7552083333333334</v>
       </c>
       <c r="E41">
-        <v>0.7552083333333334</v>
-      </c>
-      <c r="F41">
         <v>0.6858638743455497</v>
       </c>
     </row>
@@ -1282,12 +1157,9 @@
         <v>78.14285714285714</v>
       </c>
       <c r="D42">
-        <v>171357</v>
+        <v>0.675531914893617</v>
       </c>
       <c r="E42">
-        <v>0.675531914893617</v>
-      </c>
-      <c r="F42">
         <v>0.6296296296296297</v>
       </c>
     </row>
@@ -1304,12 +1176,9 @@
         <v>310.4285714285714</v>
       </c>
       <c r="D43">
-        <v>144941</v>
+        <v>0.9162303664921466</v>
       </c>
       <c r="E43">
-        <v>0.9162303664921466</v>
-      </c>
-      <c r="F43">
         <v>0.7789473684210526</v>
       </c>
     </row>
@@ -1326,12 +1195,9 @@
         <v>101</v>
       </c>
       <c r="D44">
-        <v>9780</v>
+        <v>0.7789473684210526</v>
       </c>
       <c r="E44">
-        <v>0.7789473684210526</v>
-      </c>
-      <c r="F44">
         <v>0.6808510638297872</v>
       </c>
     </row>
@@ -1348,12 +1214,9 @@
         <v>123.5714285714286</v>
       </c>
       <c r="D45">
-        <v>39528</v>
+        <v>0.9947916666666666</v>
       </c>
       <c r="E45">
-        <v>0.9947916666666666</v>
-      </c>
-      <c r="F45">
         <v>0.9479166666666666</v>
       </c>
     </row>
@@ -1370,12 +1233,9 @@
         <v>186.7142857142857</v>
       </c>
       <c r="D46">
-        <v>92619</v>
+        <v>0.1588785046728972</v>
       </c>
       <c r="E46">
-        <v>0.1588785046728972</v>
-      </c>
-      <c r="F46">
         <v>0.3565217391304348</v>
       </c>
     </row>
@@ -1392,12 +1252,9 @@
         <v>89.42857142857143</v>
       </c>
       <c r="D47">
-        <v>93627</v>
+        <v>0.8429319371727748</v>
       </c>
       <c r="E47">
-        <v>0.8429319371727748</v>
-      </c>
-      <c r="F47">
         <v>0.7083333333333334</v>
       </c>
     </row>
@@ -1414,12 +1271,9 @@
         <v>43.28571428571428</v>
       </c>
       <c r="D48">
-        <v>77090</v>
+        <v>0.7172774869109948</v>
       </c>
       <c r="E48">
-        <v>0.7172774869109948</v>
-      </c>
-      <c r="F48">
         <v>0.6631578947368421</v>
       </c>
     </row>
@@ -1436,12 +1290,9 @@
         <v>60.42857142857143</v>
       </c>
       <c r="D49">
-        <v>30126</v>
+        <v>0.6526315789473685</v>
       </c>
       <c r="E49">
-        <v>0.6526315789473685</v>
-      </c>
-      <c r="F49">
         <v>0.5925925925925926</v>
       </c>
     </row>
@@ -1458,12 +1309,9 @@
         <v>34.42857142857143</v>
       </c>
       <c r="D50">
-        <v>176889</v>
+        <v>0.837696335078534</v>
       </c>
       <c r="E50">
-        <v>0.837696335078534</v>
-      </c>
-      <c r="F50">
         <v>0.7277486910994765</v>
       </c>
     </row>
@@ -1480,12 +1328,9 @@
         <v>31.71428571428572</v>
       </c>
       <c r="D51">
-        <v>3172</v>
+        <v>0.6797752808988764</v>
       </c>
       <c r="E51">
-        <v>0.6797752808988764</v>
-      </c>
-      <c r="F51">
         <v>0.5714285714285714</v>
       </c>
     </row>
@@ -1502,12 +1347,9 @@
         <v>28.71428571428572</v>
       </c>
       <c r="D52">
-        <v>36056</v>
+        <v>0.8105263157894737</v>
       </c>
       <c r="E52">
-        <v>0.8105263157894737</v>
-      </c>
-      <c r="F52">
         <v>0.7421052631578947</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update data for LSM-analysis with new df "all_files_01_2024"
</commit_message>
<xml_diff>
--- a/RData/data_acc_cond.xlsx
+++ b/RData/data_acc_cond.xlsx
@@ -365,7 +365,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>age</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -406,951 +406,951 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>sub 4002</t>
+          <t>sub 3058</t>
         </is>
       </c>
       <c r="B3">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C3">
-        <v>185.2857142857143</v>
+        <v>1422.428571428571</v>
       </c>
       <c r="D3">
-        <v>0.2670157068062827</v>
+        <v>0.7526881720430108</v>
       </c>
       <c r="E3">
-        <v>0.2894736842105263</v>
+        <v>0.6440677966101694</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>sub 3676</t>
+          <t>sub 2917</t>
         </is>
       </c>
       <c r="B4">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C4">
-        <v>280.8571428571428</v>
+        <v>450.8571428571428</v>
       </c>
       <c r="D4">
-        <v>0.8</v>
+        <v>0.9895833333333334</v>
       </c>
       <c r="E4">
-        <v>0.7671957671957672</v>
+        <v>0.8723404255319149</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>sub 3364</t>
+          <t>sub 3104</t>
         </is>
       </c>
       <c r="B5">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="C5">
-        <v>334.4285714285714</v>
+        <v>405.5714285714286</v>
       </c>
       <c r="D5">
-        <v>0.08376963350785341</v>
+        <v>0.7684210526315789</v>
       </c>
       <c r="E5">
-        <v>0.3315508021390374</v>
+        <v>0.7315789473684211</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>sub 3299</t>
+          <t>sub 3889</t>
         </is>
       </c>
       <c r="B6">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C6">
-        <v>509.2857142857143</v>
+        <v>202.7142857142857</v>
       </c>
       <c r="D6">
-        <v>0.9166666666666666</v>
+        <v>0.824468085106383</v>
       </c>
       <c r="E6">
-        <v>0.8138297872340425</v>
+        <v>0.7819148936170213</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>sub 2884</t>
+          <t>sub 3642</t>
         </is>
       </c>
       <c r="B7">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C7">
-        <v>516.8571428571429</v>
+        <v>275</v>
       </c>
       <c r="D7">
-        <v>0.4157894736842105</v>
+        <v>0.7894736842105263</v>
       </c>
       <c r="E7">
-        <v>0.4117647058823529</v>
+        <v>0.7604166666666666</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>sub 3396</t>
+          <t>sub 3035</t>
         </is>
       </c>
       <c r="B8">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C8">
-        <v>337.2857142857143</v>
+        <v>843.2857142857143</v>
       </c>
       <c r="D8">
-        <v>0.5789473684210527</v>
+        <v>0.7777777777777778</v>
       </c>
       <c r="E8">
-        <v>0.5578947368421052</v>
+        <v>0.6770833333333334</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>sub 2998</t>
+          <t>sub 4182</t>
         </is>
       </c>
       <c r="B9">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C9">
-        <v>469.2857142857143</v>
+        <v>146.2857142857143</v>
       </c>
       <c r="D9">
-        <v>0.06914893617021277</v>
+        <v>0.8952879581151832</v>
       </c>
       <c r="E9">
-        <v>0.1555555555555556</v>
+        <v>0.8663101604278075</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>sub 4467</t>
+          <t>sub 4137</t>
         </is>
       </c>
       <c r="B10">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C10">
-        <v>31.28571428571428</v>
+        <v>162.2857142857143</v>
       </c>
       <c r="D10">
-        <v>0.5585106382978723</v>
+        <v>0.734375</v>
       </c>
       <c r="E10">
-        <v>0.5133689839572193</v>
+        <v>0.7120418848167539</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>sub 3392</t>
+          <t>sub 3583</t>
         </is>
       </c>
       <c r="B11">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C11">
-        <v>331.1428571428572</v>
+        <v>481.5714285714286</v>
       </c>
       <c r="D11">
-        <v>0.3842105263157894</v>
+        <v>0.531578947368421</v>
       </c>
       <c r="E11">
-        <v>0.3541666666666667</v>
+        <v>0.4764397905759162</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>sub 3058</t>
+          <t>sub 4281</t>
         </is>
       </c>
       <c r="B12">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="C12">
-        <v>1422.428571428571</v>
+        <v>128.5714285714286</v>
       </c>
       <c r="D12">
-        <v>0.7553191489361702</v>
+        <v>0.774869109947644</v>
       </c>
       <c r="E12">
-        <v>0.6424581005586593</v>
+        <v>0.6613756613756614</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>sub 3960</t>
+          <t>sub 4191</t>
         </is>
       </c>
       <c r="B13">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="C13">
-        <v>239.7142857142857</v>
+        <v>131.4285714285714</v>
       </c>
       <c r="D13">
-        <v>0.5276073619631901</v>
+        <v>0.6596858638743456</v>
       </c>
       <c r="E13">
-        <v>0.4903225806451613</v>
+        <v>0.7225130890052356</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>sub 2917</t>
+          <t>sub 3201</t>
         </is>
       </c>
       <c r="B14">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C14">
-        <v>450.8571428571428</v>
+        <v>436.4285714285714</v>
       </c>
       <c r="D14">
-        <v>0.9895833333333334</v>
+        <v>0.680628272251309</v>
       </c>
       <c r="E14">
-        <v>0.8677248677248677</v>
+        <v>0.6210526315789474</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>sub 3154</t>
+          <t>sub 4275</t>
         </is>
       </c>
       <c r="B15">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="C15">
-        <v>443.1428571428572</v>
+        <v>121.5714285714286</v>
       </c>
       <c r="D15">
-        <v>0.203125</v>
+        <v>0.5668449197860963</v>
       </c>
       <c r="E15">
-        <v>0.25</v>
+        <v>0.6243386243386243</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>sub 3104</t>
+          <t>sub 4170</t>
         </is>
       </c>
       <c r="B16">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="C16">
-        <v>405.5714285714286</v>
+        <v>308</v>
       </c>
       <c r="D16">
-        <v>0.7684210526315789</v>
+        <v>0.8105263157894737</v>
       </c>
       <c r="E16">
-        <v>0.7315789473684211</v>
+        <v>0.6894736842105263</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>sub 3994</t>
+          <t>sub 3676</t>
         </is>
       </c>
       <c r="B17">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C17">
-        <v>179.8571428571429</v>
+        <v>280.8571428571428</v>
       </c>
       <c r="D17">
-        <v>0.5210526315789473</v>
+        <v>0.8</v>
       </c>
       <c r="E17">
-        <v>0.5210526315789473</v>
+        <v>0.7671957671957672</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>sub 3889</t>
+          <t>sub 4431</t>
         </is>
       </c>
       <c r="B18">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C18">
-        <v>202.7142857142857</v>
+        <v>96.71428571428571</v>
       </c>
       <c r="D18">
-        <v>0.8201058201058201</v>
+        <v>0.6701570680628273</v>
       </c>
       <c r="E18">
-        <v>0.7819148936170213</v>
+        <v>0.6117021276595744</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>sub 4086</t>
+          <t>sub 4294</t>
         </is>
       </c>
       <c r="B19">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="C19">
-        <v>141.7142857142857</v>
+        <v>107.5714285714286</v>
       </c>
       <c r="D19">
-        <v>0.02604166666666667</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E19">
-        <v>0.1368421052631579</v>
+        <v>0.6031746031746031</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>sub 3642</t>
+          <t>sub 3650</t>
         </is>
       </c>
       <c r="B20">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C20">
-        <v>275</v>
+        <v>331.5714285714286</v>
       </c>
       <c r="D20">
-        <v>0.7894736842105263</v>
+        <v>0.7513227513227513</v>
       </c>
       <c r="E20">
-        <v>0.7604166666666666</v>
+        <v>0.601063829787234</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>sub 2522</t>
+          <t>sub 4140</t>
         </is>
       </c>
       <c r="B21">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C21">
-        <v>555.8571428571429</v>
+        <v>161.7142857142857</v>
       </c>
       <c r="D21">
-        <v>0.1675392670157068</v>
+        <v>0.7368421052631579</v>
       </c>
       <c r="E21">
-        <v>0.2052631578947368</v>
+        <v>0.6648351648351648</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>sub 3035</t>
+          <t>sub 3912</t>
         </is>
       </c>
       <c r="B22">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C22">
-        <v>843.2857142857143</v>
+        <v>229.8571428571429</v>
       </c>
       <c r="D22">
-        <v>0.7777777777777778</v>
+        <v>0.6631578947368421</v>
       </c>
       <c r="E22">
-        <v>0.6770833333333334</v>
+        <v>0.6210526315789474</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>sub 4182</t>
+          <t>sub 4051</t>
         </is>
       </c>
       <c r="B23">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C23">
-        <v>146.2857142857143</v>
+        <v>196.7142857142857</v>
       </c>
       <c r="D23">
-        <v>0.8952879581151832</v>
+        <v>0.8109756097560976</v>
       </c>
       <c r="E23">
-        <v>0.8663101604278075</v>
+        <v>0.632</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>sub 4137</t>
+          <t>sub 3286</t>
         </is>
       </c>
       <c r="B24">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="C24">
-        <v>162.2857142857143</v>
+        <v>390.1428571428572</v>
       </c>
       <c r="D24">
-        <v>0.734375</v>
+        <v>0.8691099476439791</v>
       </c>
       <c r="E24">
-        <v>0.7120418848167539</v>
+        <v>0.8148148148148148</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>sub 3583</t>
+          <t>sub 4208</t>
         </is>
       </c>
       <c r="B25">
         <v>51</v>
       </c>
       <c r="C25">
-        <v>481.5714285714286</v>
+        <v>137.2857142857143</v>
       </c>
       <c r="D25">
-        <v>0.531578947368421</v>
+        <v>0.78125</v>
       </c>
       <c r="E25">
-        <v>0.4764397905759162</v>
+        <v>0.7120418848167539</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>sub 4281</t>
+          <t>sub 1536</t>
         </is>
       </c>
       <c r="B26">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="C26">
-        <v>128.5714285714286</v>
+        <v>1061</v>
       </c>
       <c r="D26">
-        <v>0.774869109947644</v>
+        <v>0.6842105263157895</v>
       </c>
       <c r="E26">
-        <v>0.6613756613756614</v>
+        <v>0.6421052631578947</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>sub 4191</t>
+          <t>sub 4439</t>
         </is>
       </c>
       <c r="B27">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C27">
-        <v>131.4285714285714</v>
+        <v>79.14285714285714</v>
       </c>
       <c r="D27">
-        <v>0.6596858638743456</v>
+        <v>0.746031746031746</v>
       </c>
       <c r="E27">
-        <v>0.7225130890052356</v>
+        <v>0.6455026455026455</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>sub 3201</t>
+          <t>sub 4466</t>
         </is>
       </c>
       <c r="B28">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="C28">
-        <v>436.4285714285714</v>
+        <v>95.85714285714286</v>
       </c>
       <c r="D28">
-        <v>0.680628272251309</v>
+        <v>0.7552083333333334</v>
       </c>
       <c r="E28">
-        <v>0.6210526315789474</v>
+        <v>0.6858638743455497</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>sub 4275</t>
+          <t>sub 4504</t>
         </is>
       </c>
       <c r="B29">
         <v>55</v>
       </c>
       <c r="C29">
-        <v>121.5714285714286</v>
+        <v>78.14285714285714</v>
       </c>
       <c r="D29">
-        <v>0.5668449197860963</v>
+        <v>0.675531914893617</v>
       </c>
       <c r="E29">
-        <v>0.6243386243386243</v>
+        <v>0.6296296296296297</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>sub 4170</t>
+          <t>sub 3887</t>
         </is>
       </c>
       <c r="B30">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="C30">
-        <v>308</v>
+        <v>310.4285714285714</v>
       </c>
       <c r="D30">
-        <v>0.8105263157894737</v>
+        <v>0.9162303664921466</v>
       </c>
       <c r="E30">
-        <v>0.6894736842105263</v>
+        <v>0.7789473684210526</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>sub 4431</t>
+          <t>sub 4391</t>
         </is>
       </c>
       <c r="B31">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C31">
-        <v>96.71428571428571</v>
+        <v>101</v>
       </c>
       <c r="D31">
-        <v>0.6701570680628273</v>
+        <v>0.7789473684210526</v>
       </c>
       <c r="E31">
-        <v>0.6117021276595744</v>
+        <v>0.6808510638297872</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>sub 4294</t>
+          <t>sub 4546</t>
         </is>
       </c>
       <c r="B32">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="C32">
-        <v>107.5714285714286</v>
+        <v>123.5714285714286</v>
       </c>
       <c r="D32">
-        <v>0.6666666666666666</v>
+        <v>0.9947916666666666</v>
       </c>
       <c r="E32">
-        <v>0.6031746031746031</v>
+        <v>0.9479166666666666</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>sub 3650</t>
+          <t>sub 4227</t>
         </is>
       </c>
       <c r="B33">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="C33">
-        <v>331.5714285714286</v>
+        <v>186.7142857142857</v>
       </c>
       <c r="D33">
-        <v>0.7513227513227513</v>
+        <v>0.1588785046728972</v>
       </c>
       <c r="E33">
-        <v>0.601063829787234</v>
+        <v>0.3565217391304348</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>sub 4140</t>
+          <t>sub 4532</t>
         </is>
       </c>
       <c r="B34">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="C34">
-        <v>161.7142857142857</v>
+        <v>89.42857142857143</v>
       </c>
       <c r="D34">
-        <v>0.7368421052631579</v>
+        <v>0.8429319371727748</v>
       </c>
       <c r="E34">
-        <v>0.6648351648351648</v>
+        <v>0.7083333333333334</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>sub 3912</t>
+          <t>sub 3299</t>
         </is>
       </c>
       <c r="B35">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C35">
-        <v>229.8571428571429</v>
+        <v>509.2857142857143</v>
       </c>
       <c r="D35">
-        <v>0.6631578947368421</v>
+        <v>0.9166666666666666</v>
       </c>
       <c r="E35">
-        <v>0.6210526315789474</v>
+        <v>0.8138297872340425</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>sub 4051</t>
+          <t>sub 4720</t>
         </is>
       </c>
       <c r="B36">
         <v>59</v>
       </c>
       <c r="C36">
-        <v>196.7142857142857</v>
+        <v>43.28571428571428</v>
       </c>
       <c r="D36">
-        <v>0.8109756097560976</v>
+        <v>0.7172774869109948</v>
       </c>
       <c r="E36">
-        <v>0.632</v>
+        <v>0.6631578947368421</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>sub 3286</t>
+          <t>sub 4607</t>
         </is>
       </c>
       <c r="B37">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C37">
-        <v>390.1428571428572</v>
+        <v>60.42857142857143</v>
       </c>
       <c r="D37">
-        <v>0.8697916666666666</v>
+        <v>0.6526315789473685</v>
       </c>
       <c r="E37">
-        <v>0.8157894736842105</v>
+        <v>0.5925925925925926</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>sub 4208</t>
+          <t>sub 4728</t>
         </is>
       </c>
       <c r="B38">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C38">
-        <v>137.2857142857143</v>
+        <v>34.42857142857143</v>
       </c>
       <c r="D38">
-        <v>0.78125</v>
+        <v>0.837696335078534</v>
       </c>
       <c r="E38">
-        <v>0.7120418848167539</v>
+        <v>0.7277486910994765</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>sub 1536</t>
+          <t>sub 4769</t>
         </is>
       </c>
       <c r="B39">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="C39">
-        <v>1061</v>
+        <v>31.71428571428572</v>
       </c>
       <c r="D39">
-        <v>0.6842105263157895</v>
+        <v>0.6797752808988764</v>
       </c>
       <c r="E39">
-        <v>0.6421052631578947</v>
+        <v>0.5689655172413793</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>sub 4439</t>
+          <t>sub 4777</t>
         </is>
       </c>
       <c r="B40">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C40">
-        <v>79.14285714285714</v>
+        <v>28.71428571428572</v>
       </c>
       <c r="D40">
-        <v>0.746031746031746</v>
+        <v>0.8105263157894737</v>
       </c>
       <c r="E40">
-        <v>0.6455026455026455</v>
+        <v>0.7421052631578947</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>sub 4466</t>
+          <t>sub 3396</t>
         </is>
       </c>
       <c r="B41">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C41">
-        <v>95.85714285714286</v>
+        <v>337.2857142857143</v>
       </c>
       <c r="D41">
-        <v>0.7552083333333334</v>
+        <v>0.5789473684210527</v>
       </c>
       <c r="E41">
-        <v>0.6858638743455497</v>
+        <v>0.5578947368421052</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>sub 4504</t>
+          <t>sub 4467</t>
         </is>
       </c>
       <c r="B42">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C42">
-        <v>78.14285714285714</v>
+        <v>31.28571428571428</v>
       </c>
       <c r="D42">
-        <v>0.675531914893617</v>
+        <v>0.5585106382978723</v>
       </c>
       <c r="E42">
-        <v>0.6296296296296297</v>
+        <v>0.510752688172043</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>sub 3887</t>
+          <t>sub 3392</t>
         </is>
       </c>
       <c r="B43">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="C43">
-        <v>310.4285714285714</v>
+        <v>331.1428571428572</v>
       </c>
       <c r="D43">
-        <v>0.9162303664921466</v>
+        <v>0.6157894736842106</v>
       </c>
       <c r="E43">
-        <v>0.7789473684210526</v>
+        <v>0.6458333333333334</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>sub 4391</t>
+          <t>sub 3960</t>
         </is>
       </c>
       <c r="B44">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="C44">
-        <v>101</v>
+        <v>239.7142857142857</v>
       </c>
       <c r="D44">
-        <v>0.7789473684210526</v>
+        <v>0.4658385093167702</v>
       </c>
       <c r="E44">
-        <v>0.6808510638297872</v>
+        <v>0.5098039215686274</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>sub 4546</t>
+          <t>sub 3154</t>
         </is>
       </c>
       <c r="B45">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C45">
-        <v>123.5714285714286</v>
+        <v>443.1428571428572</v>
       </c>
       <c r="D45">
-        <v>0.9947916666666666</v>
+        <v>0.796875</v>
       </c>
       <c r="E45">
-        <v>0.9479166666666666</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>sub 4227</t>
+          <t>sub 3994</t>
         </is>
       </c>
       <c r="B46">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="C46">
-        <v>186.7142857142857</v>
+        <v>179.8571428571429</v>
       </c>
       <c r="D46">
-        <v>0.1588785046728972</v>
+        <v>0.4789473684210526</v>
       </c>
       <c r="E46">
-        <v>0.3565217391304348</v>
+        <v>0.4789473684210526</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>sub 4532</t>
+          <t>sub 4086</t>
         </is>
       </c>
       <c r="B47">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C47">
-        <v>89.42857142857143</v>
+        <v>141.7142857142857</v>
       </c>
       <c r="D47">
-        <v>0.8429319371727748</v>
+        <v>0.9739583333333334</v>
       </c>
       <c r="E47">
-        <v>0.7083333333333334</v>
+        <v>0.8631578947368421</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>sub 4720</t>
+          <t>sub 4002</t>
         </is>
       </c>
       <c r="B48">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C48">
-        <v>43.28571428571428</v>
+        <v>185.2857142857143</v>
       </c>
       <c r="D48">
-        <v>0.7172774869109948</v>
+        <v>0.7368421052631579</v>
       </c>
       <c r="E48">
-        <v>0.6631578947368421</v>
+        <v>0.7105263157894737</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>sub 4607</t>
+          <t>sub 2522</t>
         </is>
       </c>
       <c r="B49">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="C49">
-        <v>60.42857142857143</v>
+        <v>555.8571428571429</v>
       </c>
       <c r="D49">
-        <v>0.6526315789473685</v>
+        <v>0.8324607329842932</v>
       </c>
       <c r="E49">
-        <v>0.5925925925925926</v>
+        <v>0.7947368421052632</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>sub 4728</t>
+          <t>sub 3364</t>
         </is>
       </c>
       <c r="B50">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C50">
-        <v>34.42857142857143</v>
+        <v>334.4285714285714</v>
       </c>
       <c r="D50">
-        <v>0.837696335078534</v>
+        <v>0.9162303664921466</v>
       </c>
       <c r="E50">
-        <v>0.7277486910994765</v>
+        <v>0.6684491978609626</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>sub 4769</t>
+          <t>sub 2884</t>
         </is>
       </c>
       <c r="B51">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C51">
-        <v>31.71428571428572</v>
+        <v>516.8571428571429</v>
       </c>
       <c r="D51">
-        <v>0.6797752808988764</v>
+        <v>0.5842105263157895</v>
       </c>
       <c r="E51">
-        <v>0.5714285714285714</v>
+        <v>0.5882352941176471</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>sub 4777</t>
+          <t>sub 2998</t>
         </is>
       </c>
       <c r="B52">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C52">
-        <v>28.71428571428572</v>
+        <v>469.2857142857143</v>
       </c>
       <c r="D52">
-        <v>0.8105263157894737</v>
+        <v>0.9304812834224599</v>
       </c>
       <c r="E52">
-        <v>0.7421052631578947</v>
+        <v>0.848314606741573</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New .csv- and .xlsx-data files with subsample n = 41
</commit_message>
<xml_diff>
--- a/RData/data_acc_cond.xlsx
+++ b/RData/data_acc_cond.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1163,196 +1163,6 @@
         <v>0.510752688172043</v>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>sub 3392</t>
-        </is>
-      </c>
-      <c r="B43">
-        <v>53</v>
-      </c>
-      <c r="C43">
-        <v>331.1428571428572</v>
-      </c>
-      <c r="D43">
-        <v>0.6157894736842106</v>
-      </c>
-      <c r="E43">
-        <v>0.6458333333333334</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>sub 3960</t>
-        </is>
-      </c>
-      <c r="B44">
-        <v>79</v>
-      </c>
-      <c r="C44">
-        <v>239.7142857142857</v>
-      </c>
-      <c r="D44">
-        <v>0.4658385093167702</v>
-      </c>
-      <c r="E44">
-        <v>0.5098039215686274</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>sub 3154</t>
-        </is>
-      </c>
-      <c r="B45">
-        <v>30</v>
-      </c>
-      <c r="C45">
-        <v>443.1428571428572</v>
-      </c>
-      <c r="D45">
-        <v>0.796875</v>
-      </c>
-      <c r="E45">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>sub 3994</t>
-        </is>
-      </c>
-      <c r="B46">
-        <v>55</v>
-      </c>
-      <c r="C46">
-        <v>179.8571428571429</v>
-      </c>
-      <c r="D46">
-        <v>0.4789473684210526</v>
-      </c>
-      <c r="E46">
-        <v>0.4789473684210526</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>sub 4086</t>
-        </is>
-      </c>
-      <c r="B47">
-        <v>59</v>
-      </c>
-      <c r="C47">
-        <v>141.7142857142857</v>
-      </c>
-      <c r="D47">
-        <v>0.9739583333333334</v>
-      </c>
-      <c r="E47">
-        <v>0.8631578947368421</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>sub 4002</t>
-        </is>
-      </c>
-      <c r="B48">
-        <v>69</v>
-      </c>
-      <c r="C48">
-        <v>185.2857142857143</v>
-      </c>
-      <c r="D48">
-        <v>0.7368421052631579</v>
-      </c>
-      <c r="E48">
-        <v>0.7105263157894737</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>sub 2522</t>
-        </is>
-      </c>
-      <c r="B49">
-        <v>40</v>
-      </c>
-      <c r="C49">
-        <v>555.8571428571429</v>
-      </c>
-      <c r="D49">
-        <v>0.8324607329842932</v>
-      </c>
-      <c r="E49">
-        <v>0.7947368421052632</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>sub 3364</t>
-        </is>
-      </c>
-      <c r="B50">
-        <v>34</v>
-      </c>
-      <c r="C50">
-        <v>334.4285714285714</v>
-      </c>
-      <c r="D50">
-        <v>0.9162303664921466</v>
-      </c>
-      <c r="E50">
-        <v>0.6684491978609626</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>sub 2884</t>
-        </is>
-      </c>
-      <c r="B51">
-        <v>55</v>
-      </c>
-      <c r="C51">
-        <v>516.8571428571429</v>
-      </c>
-      <c r="D51">
-        <v>0.5842105263157895</v>
-      </c>
-      <c r="E51">
-        <v>0.5882352941176471</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>sub 2998</t>
-        </is>
-      </c>
-      <c r="B52">
-        <v>59</v>
-      </c>
-      <c r="C52">
-        <v>469.2857142857143</v>
-      </c>
-      <c r="D52">
-        <v>0.9304812834224599</v>
-      </c>
-      <c r="E52">
-        <v>0.848314606741573</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>